<commit_message>
update: replay buffer save
</commit_message>
<xml_diff>
--- a/scenario_data.xlsx
+++ b/scenario_data.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="scenario_3_RL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="scenario_1_RL" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -448,7 +448,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>33.59</t>
+          <t>62.25</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.34</t>
+          <t>1.19</t>
         </is>
       </c>
     </row>
@@ -472,7 +472,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3.36</t>
+          <t>3.74</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>